<commit_message>
Cambios a la planeación
</commit_message>
<xml_diff>
--- a/Planeacion_Sistema.xlsx
+++ b/Planeacion_Sistema.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Lista de actividades</t>
   </si>
@@ -49,6 +49,18 @@
   </si>
   <si>
     <t>Todos</t>
+  </si>
+  <si>
+    <t>Fecha de entrega:</t>
+  </si>
+  <si>
+    <t>Encargado de comunicación</t>
+  </si>
+  <si>
+    <t>Fecha de revisión:</t>
+  </si>
+  <si>
+    <t>Encargado de revisiones</t>
   </si>
 </sst>
 </file>
@@ -387,26 +399,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -414,39 +436,49 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizando versiones de actividades y planeación, Jesús
</commit_message>
<xml_diff>
--- a/Planeacion_Sistema.xlsx
+++ b/Planeacion_Sistema.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Lista de actividades</t>
   </si>
@@ -27,24 +27,12 @@
     <t>Pantallas del sistema:</t>
   </si>
   <si>
-    <t>Inicio de sesión</t>
-  </si>
-  <si>
     <t>Creación de la BD</t>
   </si>
   <si>
     <t>Llenado de la BD</t>
   </si>
   <si>
-    <t>Vista de carga de horarios</t>
-  </si>
-  <si>
-    <t>Vista de validación de horarios</t>
-  </si>
-  <si>
-    <t>Vista de horarios de materias</t>
-  </si>
-  <si>
     <t>Responsable:</t>
   </si>
   <si>
@@ -100,6 +88,36 @@
   </si>
   <si>
     <t>Horario máximo 11pm</t>
+  </si>
+  <si>
+    <t>Vista de actualizar de horario (altas, bajas, cambios)</t>
+  </si>
+  <si>
+    <t>Domingo 3 de mayo</t>
+  </si>
+  <si>
+    <t>Domingo 10 de mayo</t>
+  </si>
+  <si>
+    <t>Domingo 17 de mayo</t>
+  </si>
+  <si>
+    <t>Domingo 24 de mayo</t>
+  </si>
+  <si>
+    <t>Vista de validación de horarios (administrador)</t>
+  </si>
+  <si>
+    <t>Vista de horarios de materias (maestros)</t>
+  </si>
+  <si>
+    <t>Inicio de sesión (maestros, administrador)</t>
+  </si>
+  <si>
+    <t>Documentación</t>
+  </si>
+  <si>
+    <t>Fecha final:</t>
   </si>
 </sst>
 </file>
@@ -438,15 +456,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="46.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
@@ -459,19 +477,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -479,12 +497,12 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -494,77 +512,142 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>